<commit_message>
Mise à jour 0.0.2 - Ajout de classes de base
*Ajout de la classe Équipement
*Ajout de la classe Inventaire
*Ajout de la classe Caractéristiques
*Ajout de la classe Ennemi
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit1.xlsx
+++ b/Audits/sommaireAudit1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>No tâche</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Partir les scripts</t>
+  </si>
+  <si>
+    <t>Anthony Gauthier, Tommy Gingras</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -537,8 +540,8 @@
         <v>17</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E2" s="4">
         <v>3</v>

</xml_diff>

<commit_message>
Mise à jour BD, Sommaire, Specs
Insertion armes, specs ajoutées
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit1.xlsx
+++ b/Audits/sommaireAudit1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>No tâche</t>
   </si>
@@ -102,18 +102,9 @@
     <t>Attribué</t>
   </si>
   <si>
-    <t>Personnalisation des caractéristiques</t>
-  </si>
-  <si>
-    <t>Choix du visuel</t>
-  </si>
-  <si>
     <t>Image du personnage</t>
   </si>
   <si>
-    <t>Choix de la profession et du nom</t>
-  </si>
-  <si>
     <t>Création d'image de personnage</t>
   </si>
   <si>
@@ -129,16 +120,19 @@
     <t>Création de l'écran «Changement de personnage»</t>
   </si>
   <si>
-    <t>Création de la base de données</t>
-  </si>
-  <si>
-    <t>Partir les scripts</t>
-  </si>
-  <si>
     <t>Anthony Gauthier, Tommy Gingras</t>
   </si>
   <si>
     <t>Coordination</t>
+  </si>
+  <si>
+    <t>Fonctionnalité choix du visuel</t>
+  </si>
+  <si>
+    <t>Fonctionnalité personnalisation des caractéristiques</t>
+  </si>
+  <si>
+    <t>Fonctionnalité choix de la profession et du nom</t>
   </si>
 </sst>
 </file>
@@ -501,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
@@ -544,7 +538,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E2" s="4">
         <v>3</v>
@@ -568,145 +562,146 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f t="shared" ref="A5:A18" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <f t="shared" ref="A6:A19" si="0">A5+1</f>
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E6" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E9" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>27</v>
@@ -715,36 +710,36 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>27</v>
@@ -753,10 +748,10 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -772,12 +767,14 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
         <v>8</v>
       </c>
@@ -791,14 +788,12 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
         <v>8</v>
       </c>
@@ -810,35 +805,35 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>27</v>
@@ -846,18 +841,18 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f>A16+1</f>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E18" s="4">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>27</v>
@@ -865,50 +860,39 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="4">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="4">
-        <v>3</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
+        <f>SUM(E2:E19)</f>
+        <v>94.5</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4">
-        <f>SUM(E2:E20)</f>
-        <v>82</v>
-      </c>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,33 +915,25 @@
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mise à jour 0.0.5
*Ajout de l'écran de choix de personnage
*Ajout de quelques champs (hp,mana, niveau, nom perso)
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit1.xlsx
+++ b/Audits/sommaireAudit1.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,6 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -570,7 +569,6 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -589,7 +587,6 @@
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f t="shared" ref="A5:A18" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -610,7 +607,6 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -629,7 +625,6 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -650,7 +645,6 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -669,7 +663,6 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -690,7 +683,6 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -709,7 +701,6 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -728,7 +719,6 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -747,7 +737,6 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -766,7 +755,6 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -787,7 +775,6 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -805,7 +792,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
@@ -822,8 +811,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f>A15+1</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>32</v>
@@ -841,8 +829,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
@@ -860,7 +847,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Modification classe Joueurs et VarGlobales
J'ai corrigé l'accès au joueur
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit1.xlsx
+++ b/Audits/sommaireAudit1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>No tâche</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Fonctionnalité choix de la profession et du nom</t>
+  </si>
+  <si>
+    <t>permet la création d'un personnage</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -248,7 +302,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,7 +337,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,10 +668,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -669,13 +723,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -721,7 +775,9 @@
       <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
@@ -729,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -739,7 +795,9 @@
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
@@ -747,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,7 +925,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4">
         <f>SUM(E2:E19)</f>
-        <v>94.5</v>
+        <v>86</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -920,6 +978,24 @@
       <c r="F26" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:F2">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:F19">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>